<commit_message>
NN + backend files get post
</commit_message>
<xml_diff>
--- a/utils/results.xlsx
+++ b/utils/results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programs\Poteem\easy-knowledge\gpt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programs\Poteem\easy-knowledge\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E8F96E1F-50C3-4FC5-962D-422A64238157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DD703F3-72AD-4F0E-8342-BD3EFF65D6A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{88C3A490-32D0-4B56-A966-8D0208257156}"/>
+    <workbookView xWindow="10215" yWindow="960" windowWidth="18330" windowHeight="15090" xr2:uid="{88C3A490-32D0-4B56-A966-8D0208257156}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
   <si>
     <t>price</t>
   </si>
@@ -55,6 +55,18 @@
   </si>
   <si>
     <t>sum</t>
+  </si>
+  <si>
+    <t>money limit</t>
+  </si>
+  <si>
+    <t>total price per token</t>
+  </si>
+  <si>
+    <t>tk output rate</t>
+  </si>
+  <si>
+    <t>max amount of input tokens</t>
   </si>
 </sst>
 </file>
@@ -413,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F9B91B-06D2-4857-A529-EFB98C42BE8B}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.42578125" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -424,7 +436,11 @@
     <col min="1" max="2" width="12.140625" style="1" customWidth="1"/>
     <col min="3" max="4" width="10.42578125" style="1"/>
     <col min="5" max="5" width="13.140625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.42578125" style="1"/>
+    <col min="6" max="6" width="10.42578125" style="1"/>
+    <col min="7" max="7" width="19.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -482,10 +498,12 @@
       <c r="G4" s="1">
         <v>785</v>
       </c>
-      <c r="H4" s="1">
+    </row>
+    <row r="5" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H5" s="1">
         <v>3498</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I5" s="1">
         <v>534</v>
       </c>
     </row>
@@ -524,12 +542,12 @@
         <v>1.57E-3</v>
       </c>
       <c r="C9" s="1">
-        <f>H4/1000*A3</f>
-        <v>3.4980000000000002E-3</v>
+        <f>H$4/1000*A3</f>
+        <v>0</v>
       </c>
       <c r="D9" s="1">
-        <f>I4/1000*B3</f>
-        <v>1.0680000000000002E-3</v>
+        <f>I$4/1000*B3</f>
+        <v>0</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>7</v>
@@ -546,25 +564,56 @@
       </c>
       <c r="C10" s="1">
         <f t="shared" si="0"/>
-        <v>0.67161599999999999</v>
+        <v>0</v>
       </c>
       <c r="D10" s="1">
         <f t="shared" si="0"/>
-        <v>0.20505600000000002</v>
+        <v>0</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="G12" s="1">
+        <f>(G4)/F4</f>
+        <v>0.19488579940417081</v>
+      </c>
+      <c r="H12" s="1">
+        <v>2</v>
+      </c>
+      <c r="I12" s="1">
+        <f>H12/G14*1000</f>
+        <v>1439085.3876384425</v>
+      </c>
     </row>
     <row r="13" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <f>SUM(A10:D10)</f>
-        <v>1.9514879999999999</v>
+        <v>1.0748159999999998</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G14" s="1">
+        <f>A3+B3*G12</f>
+        <v>1.3897715988083416E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>